<commit_message>
20250814 - API Search Attempt
</commit_message>
<xml_diff>
--- a/GUI + Reviews/Review Comparison/index_comparison_results_20250812_131342.xlsx
+++ b/GUI + Reviews/Review Comparison/index_comparison_results_20250812_131342.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/Review Comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_D6E23D0399BE47862E712E943AE5A9C5506C23ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24B66859-59E9-4CDE-A321-762C8A9A1474}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_D6E23D0399BE47862E712E943AE5A9C5506C23ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{777D6B90-EBE1-4D98-84FD-883CBD1E9FB3}"/>
   <bookViews>
-    <workbookView xWindow="-29370" yWindow="195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -3450,7 +3450,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3614,7 +3616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>